<commit_message>
Codigo Generador de Ondas
</commit_message>
<xml_diff>
--- a/Codigos Antiguos/Bioimpedanciometro_Sketch_Funcional_3.0/Datos Bioimpedanciometro.xlsx
+++ b/Codigos Antiguos/Bioimpedanciometro_Sketch_Funcional_3.0/Datos Bioimpedanciometro.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Documents\GitHub\Programaci-n-con-Arduino\Bioimpedanciometro_Sketch_Funcional_3.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Documents\GitHub\Programaci-n-con-Arduino\Codigos Antiguos\Bioimpedanciometro_Sketch_Funcional_3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja4" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
     <sheet name="Hoja5" sheetId="5" r:id="rId5"/>
     <sheet name="Hoja6" sheetId="6" r:id="rId6"/>
+    <sheet name="Hoja7" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Hoja2!$E$5:$F$11</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
   <si>
     <t>Valor medido</t>
   </si>
@@ -179,6 +180,30 @@
   </si>
   <si>
     <t>Error Porcentual</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Reactancia</t>
+  </si>
+  <si>
+    <t>1/Z</t>
+  </si>
+  <si>
+    <t>Serie Z</t>
+  </si>
+  <si>
+    <t>Z Teorico</t>
+  </si>
+  <si>
+    <t>Z Sensado</t>
   </si>
 </sst>
 </file>
@@ -361,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -441,6 +466,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -474,7 +503,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,7 +567,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -649,11 +678,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-841703744"/>
-        <c:axId val="-841700480"/>
+        <c:axId val="-1460971536"/>
+        <c:axId val="-1460978064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-841703744"/>
+        <c:axId val="-1460971536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -700,7 +729,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -767,12 +795,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-841700480"/>
+        <c:crossAx val="-1460978064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-841700480"/>
+        <c:axId val="-1460978064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -833,7 +861,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -900,7 +927,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-841703744"/>
+        <c:crossAx val="-1460971536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1209,11 +1236,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-775557504"/>
-        <c:axId val="-775556416"/>
+        <c:axId val="-1457690848"/>
+        <c:axId val="-1457689760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-775557504"/>
+        <c:axId val="-1457690848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1270,12 +1297,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775556416"/>
+        <c:crossAx val="-1457689760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-775556416"/>
+        <c:axId val="-1457689760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1332,7 +1359,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775557504"/>
+        <c:crossAx val="-1457690848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1561,11 +1588,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-774928032"/>
-        <c:axId val="-774931840"/>
+        <c:axId val="-1412797968"/>
+        <c:axId val="-1412796880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-774928032"/>
+        <c:axId val="-1412797968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1622,12 +1649,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-774931840"/>
+        <c:crossAx val="-1412796880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-774931840"/>
+        <c:axId val="-1412796880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1684,7 +1711,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-774928032"/>
+        <c:crossAx val="-1412797968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1913,11 +1940,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-774930208"/>
-        <c:axId val="-774927488"/>
+        <c:axId val="-1412800688"/>
+        <c:axId val="-1412807216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-774930208"/>
+        <c:axId val="-1412800688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1974,12 +2001,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-774927488"/>
+        <c:crossAx val="-1412807216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-774927488"/>
+        <c:axId val="-1412807216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2036,7 +2063,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-774930208"/>
+        <c:crossAx val="-1412800688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2114,7 +2141,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2265,11 +2291,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-774929664"/>
-        <c:axId val="-774929120"/>
+        <c:axId val="-1412806672"/>
+        <c:axId val="-1412804496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-774929664"/>
+        <c:axId val="-1412806672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2326,12 +2352,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-774929120"/>
+        <c:crossAx val="-1412804496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-774929120"/>
+        <c:axId val="-1412804496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2388,7 +2414,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-774929664"/>
+        <c:crossAx val="-1412806672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2663,11 +2689,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-773917680"/>
-        <c:axId val="-773919312"/>
+        <c:axId val="-1412806128"/>
+        <c:axId val="-1412805584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-773917680"/>
+        <c:axId val="-1412806128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2760,12 +2786,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773919312"/>
+        <c:crossAx val="-1412805584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-773919312"/>
+        <c:axId val="-1412805584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2858,7 +2884,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773917680"/>
+        <c:crossAx val="-1412806128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2936,7 +2962,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3114,11 +3139,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-773910064"/>
-        <c:axId val="-773923664"/>
+        <c:axId val="-1412801776"/>
+        <c:axId val="-1412800144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-773910064"/>
+        <c:axId val="-1412801776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3170,12 +3195,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773923664"/>
+        <c:crossAx val="-1412800144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-773923664"/>
+        <c:axId val="-1412800144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3231,7 +3256,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773910064"/>
+        <c:crossAx val="-1412801776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3298,7 +3323,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3476,11 +3500,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-773922576"/>
-        <c:axId val="-773909520"/>
+        <c:axId val="-1412799600"/>
+        <c:axId val="-1412799056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-773922576"/>
+        <c:axId val="-1412799600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3532,12 +3556,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773909520"/>
+        <c:crossAx val="-1412799056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-773909520"/>
+        <c:axId val="-1412799056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3593,7 +3617,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773922576"/>
+        <c:crossAx val="-1412799600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3660,7 +3684,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3838,11 +3861,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-773920944"/>
-        <c:axId val="-773920400"/>
+        <c:axId val="-1412793072"/>
+        <c:axId val="-1412792528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-773920944"/>
+        <c:axId val="-1412793072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3894,12 +3917,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773920400"/>
+        <c:crossAx val="-1412792528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-773920400"/>
+        <c:axId val="-1412792528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3955,7 +3978,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773920944"/>
+        <c:crossAx val="-1412793072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4022,7 +4045,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4200,11 +4222,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-773916048"/>
-        <c:axId val="-773917136"/>
+        <c:axId val="-1411819136"/>
+        <c:axId val="-1411825664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-773916048"/>
+        <c:axId val="-1411819136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4256,12 +4278,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773917136"/>
+        <c:crossAx val="-1411825664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-773917136"/>
+        <c:axId val="-1411825664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4317,7 +4339,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773916048"/>
+        <c:crossAx val="-1411819136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4579,11 +4601,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-841698848"/>
-        <c:axId val="-841698304"/>
+        <c:axId val="-1460972080"/>
+        <c:axId val="-1460970992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-841698848"/>
+        <c:axId val="-1460972080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4626,7 +4648,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-841698304"/>
+        <c:crossAx val="-1460970992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4634,7 +4656,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-841698304"/>
+        <c:axId val="-1460970992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4685,7 +4707,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-841698848"/>
+        <c:crossAx val="-1460972080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4961,11 +4983,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-875209696"/>
-        <c:axId val="-775561856"/>
+        <c:axId val="-1644680272"/>
+        <c:axId val="-1457690304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-875209696"/>
+        <c:axId val="-1644680272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5008,7 +5030,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775561856"/>
+        <c:crossAx val="-1457690304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5016,7 +5038,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-775561856"/>
+        <c:axId val="-1457690304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5067,7 +5089,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-875209696"/>
+        <c:crossAx val="-1644680272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5351,11 +5373,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-775552608"/>
-        <c:axId val="-775561312"/>
+        <c:axId val="-1457685408"/>
+        <c:axId val="-1457681600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-775552608"/>
+        <c:axId val="-1457685408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5407,12 +5429,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775561312"/>
+        <c:crossAx val="-1457681600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-775561312"/>
+        <c:axId val="-1457681600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5468,7 +5490,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775552608"/>
+        <c:crossAx val="-1457685408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5709,11 +5731,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-775554240"/>
-        <c:axId val="-775552064"/>
+        <c:axId val="-1457687584"/>
+        <c:axId val="-1457688672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-775554240"/>
+        <c:axId val="-1457687584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5765,12 +5787,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775552064"/>
+        <c:crossAx val="-1457688672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-775552064"/>
+        <c:axId val="-1457688672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5826,7 +5848,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775554240"/>
+        <c:crossAx val="-1457687584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6088,11 +6110,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-775553152"/>
-        <c:axId val="-775550976"/>
+        <c:axId val="-1457688128"/>
+        <c:axId val="-1457694112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-775553152"/>
+        <c:axId val="-1457688128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6144,12 +6166,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775550976"/>
+        <c:crossAx val="-1457694112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-775550976"/>
+        <c:axId val="-1457694112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6205,7 +6227,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775553152"/>
+        <c:crossAx val="-1457688128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6446,11 +6468,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-775550432"/>
-        <c:axId val="-775565664"/>
+        <c:axId val="-1457684320"/>
+        <c:axId val="-1457682144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-775550432"/>
+        <c:axId val="-1457684320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6502,12 +6524,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775565664"/>
+        <c:crossAx val="-1457682144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-775565664"/>
+        <c:axId val="-1457682144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6563,7 +6585,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775550432"/>
+        <c:crossAx val="-1457684320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6804,11 +6826,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-775559680"/>
-        <c:axId val="-775558048"/>
+        <c:axId val="-1457682688"/>
+        <c:axId val="-1457696288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-775559680"/>
+        <c:axId val="-1457682688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6860,12 +6882,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775558048"/>
+        <c:crossAx val="-1457696288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-775558048"/>
+        <c:axId val="-1457696288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6921,7 +6943,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775559680"/>
+        <c:crossAx val="-1457682688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7162,11 +7184,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-775559136"/>
-        <c:axId val="-775562944"/>
+        <c:axId val="-1457693568"/>
+        <c:axId val="-1457693024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-775559136"/>
+        <c:axId val="-1457693568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7218,12 +7240,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775562944"/>
+        <c:crossAx val="-1457693024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-775562944"/>
+        <c:axId val="-1457693024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7279,7 +7301,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-775559136"/>
+        <c:crossAx val="-1457693568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17970,20 +17992,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="40"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="22" t="s">
         <v>15</v>
       </c>
@@ -18010,7 +18032,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="24">
         <v>140</v>
       </c>
@@ -18037,7 +18059,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="24">
         <v>163</v>
       </c>
@@ -18064,7 +18086,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="24">
         <v>149</v>
       </c>
@@ -18091,7 +18113,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="24">
         <v>135</v>
       </c>
@@ -18118,7 +18140,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="24">
         <v>149</v>
       </c>
@@ -18145,7 +18167,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="24">
         <v>140</v>
       </c>
@@ -18172,7 +18194,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="24">
         <v>134</v>
       </c>
@@ -18199,7 +18221,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="24">
         <v>183</v>
       </c>
@@ -18226,7 +18248,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="24">
         <v>171</v>
       </c>
@@ -18253,7 +18275,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="24">
         <v>180</v>
       </c>
@@ -18280,7 +18302,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="24">
         <v>139</v>
       </c>
@@ -18307,7 +18329,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="26"/>
       <c r="C15" s="27"/>
       <c r="D15" s="27"/>
@@ -18320,7 +18342,7 @@
       <c r="I15" s="27"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="29">
         <f t="shared" ref="B16:I16" si="0">(B4+B5+B6+B7+B8+B9+B10+B11+B12+B13)/10</f>
         <v>154.4</v>
@@ -18518,22 +18540,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="H3" s="39" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="H3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -19100,12 +19122,12 @@
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="5" t="s">
         <v>7</v>
       </c>
@@ -19245,12 +19267,12 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
       <c r="G13" s="5" t="s">
         <v>7</v>
       </c>
@@ -19391,12 +19413,12 @@
       <c r="B21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
       <c r="G21" s="5" t="s">
         <v>7</v>
       </c>
@@ -19546,12 +19568,12 @@
       <c r="B30" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
       <c r="G30" s="5" t="s">
         <v>7</v>
       </c>
@@ -19669,7 +19691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L5" workbookViewId="0">
+    <sheetView topLeftCell="L5" workbookViewId="0">
       <selection activeCell="P11" sqref="P11:R23"/>
     </sheetView>
   </sheetViews>
@@ -19685,12 +19707,12 @@
       <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="11" t="s">
         <v>7</v>
       </c>
@@ -19800,7 +19822,7 @@
       <c r="Q11" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="R11" s="44" t="s">
+      <c r="R11" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -19823,12 +19845,12 @@
       <c r="B13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
       <c r="G13" s="11" t="s">
         <v>7</v>
       </c>
@@ -20024,12 +20046,12 @@
       <c r="B21" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
       <c r="G21" s="11" t="s">
         <v>7</v>
       </c>
@@ -20176,12 +20198,12 @@
       <c r="B29" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="11" t="s">
         <v>7</v>
       </c>
@@ -20359,7 +20381,7 @@
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="42" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3">
@@ -20412,7 +20434,7 @@
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="40"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="3">
         <v>20164</v>
       </c>
@@ -20463,7 +20485,7 @@
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="40"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="3">
         <v>20128</v>
       </c>
@@ -20514,7 +20536,7 @@
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="40"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="3">
         <v>20138</v>
       </c>
@@ -20565,7 +20587,7 @@
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="40"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="3">
         <v>20196</v>
       </c>
@@ -20616,7 +20638,7 @@
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="40"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="3">
         <v>20120</v>
       </c>
@@ -20667,7 +20689,7 @@
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="40"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="3">
         <v>20132</v>
       </c>
@@ -20718,7 +20740,7 @@
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="40"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="3">
         <v>20183</v>
       </c>
@@ -20769,7 +20791,7 @@
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="40"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="3">
         <v>20129</v>
       </c>
@@ -20820,7 +20842,7 @@
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="40"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="3">
         <v>20131</v>
       </c>
@@ -20871,7 +20893,7 @@
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="40"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="3">
         <v>20133</v>
       </c>
@@ -20922,7 +20944,7 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="40"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="3">
         <v>20181</v>
       </c>
@@ -20973,7 +20995,7 @@
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="3">
         <v>20169</v>
       </c>
@@ -21024,7 +21046,7 @@
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="40"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="3">
         <v>20101</v>
       </c>
@@ -21075,7 +21097,7 @@
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="40"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="3">
         <v>20133</v>
       </c>
@@ -21126,7 +21148,7 @@
       </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
+      <c r="B21" s="42"/>
       <c r="C21" s="3">
         <v>20144</v>
       </c>
@@ -21177,7 +21199,7 @@
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="40"/>
+      <c r="B22" s="42"/>
       <c r="C22" s="3">
         <v>20103</v>
       </c>
@@ -21228,7 +21250,7 @@
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B23" s="40"/>
+      <c r="B23" s="42"/>
       <c r="C23" s="3">
         <v>20169</v>
       </c>
@@ -21279,7 +21301,7 @@
       </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B24" s="40"/>
+      <c r="B24" s="42"/>
       <c r="C24" s="3">
         <v>20100</v>
       </c>
@@ -21330,7 +21352,7 @@
       </c>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="40"/>
+      <c r="B25" s="42"/>
       <c r="C25" s="3">
         <v>20115</v>
       </c>
@@ -21450,7 +21472,7 @@
       </c>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="43" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="3">
@@ -21462,7 +21484,7 @@
       </c>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B30" s="42"/>
+      <c r="B30" s="44"/>
       <c r="C30" s="3">
         <f>(D6+D7+D8+D9+D10+D11+D12+D13+D14+D15+D16+D17+D18+D19+D20+D21+D22+D23+D24+D25)/20</f>
         <v>20120.8</v>
@@ -21472,7 +21494,7 @@
       </c>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B31" s="42"/>
+      <c r="B31" s="44"/>
       <c r="C31" s="3">
         <f>(E6+E7+E8+E9+E10+E11+E12+E13+E14+E15+E16+E17+E18+E19+E20+E21+E22+E23+E24+E25)/20</f>
         <v>20107.45</v>
@@ -21482,7 +21504,7 @@
       </c>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B32" s="43"/>
+      <c r="B32" s="45"/>
       <c r="C32" s="3">
         <f>(F6+F7+F8+F9+F10+F11+F12+F13+F14+F15+F16+F17+F18+F19+F20+F21+F22+F23+F24+F25)/20</f>
         <v>20084.599999999999</v>
@@ -21521,7 +21543,7 @@
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="43" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="3">
@@ -21533,7 +21555,7 @@
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="42"/>
+      <c r="B39" s="44"/>
       <c r="C39" s="3">
         <f>(I6+I7+I8+I9+I10+I11+I12+I13+I14+I15+I16+I17+I18+I19+I20+I21+I22+I23+I24+I25)/20</f>
         <v>20011.400000000001</v>
@@ -21543,7 +21565,7 @@
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="42"/>
+      <c r="B40" s="44"/>
       <c r="C40" s="3">
         <f>(J6+J7+J8+J9+J10+J11+J12+J13+J14+J15+J16+J17+J18+J19+J20+J21+J22+J23+J24+J25)/20</f>
         <v>19950.599999999999</v>
@@ -21553,7 +21575,7 @@
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="43"/>
+      <c r="B41" s="45"/>
       <c r="C41" s="3">
         <f>(K6+K7+K8+K9+K10+K11+K12+K13+K14+K15+K16+K17+K18+K19+K20+K21+K22+K23+K24+K25)/20</f>
         <v>19838.099999999999</v>
@@ -21592,7 +21614,7 @@
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="41" t="s">
+      <c r="B46" s="43" t="s">
         <v>31</v>
       </c>
       <c r="C46" s="3">
@@ -21604,7 +21626,7 @@
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="42"/>
+      <c r="B47" s="44"/>
       <c r="C47" s="3">
         <f>(N6+N7+N8+N9+N10+N11+N12+N13+N14+N15+N16+N17+N18+N19+N20+N21+N22+N23+N24+N25)/20</f>
         <v>19663.849999999999</v>
@@ -21614,7 +21636,7 @@
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="42"/>
+      <c r="B48" s="44"/>
       <c r="C48" s="3">
         <f>(O6+O7+O8+O9+O10+O11+O12+O13+O14+O15+O16+O17+O18+O19+O20+O21+O22+O23+O24+O25)/20</f>
         <v>19486.5</v>
@@ -21624,7 +21646,7 @@
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="43"/>
+      <c r="B49" s="45"/>
       <c r="C49" s="3">
         <f>(P6+P7+P8+P9+P10+P11+P12+P13+P14+P15+P16+P17+P18+P19+P20+P21+P22+P23+P24+P25)/20</f>
         <v>19472.099999999999</v>
@@ -21659,7 +21681,7 @@
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="41" t="s">
+      <c r="B54" s="43" t="s">
         <v>32</v>
       </c>
       <c r="C54" s="2">
@@ -21671,7 +21693,7 @@
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="42"/>
+      <c r="B55" s="44"/>
       <c r="C55" s="2">
         <f>(S6+S7+S8+S9+S10+S11+S12+S13+S14+S15+S16+S17+S18+S19+S20+S21+S22+S23+S24+S25)/20</f>
         <v>18965.849999999999</v>
@@ -21681,7 +21703,7 @@
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="42"/>
+      <c r="B56" s="44"/>
       <c r="C56" s="2">
         <f>(T6+T7+T8+T9+T10+T11+T12+T13+T14+T15+T16+T17+T18+T19+T20+T21+T22+T23+T24+T25)/20</f>
         <v>18418.45</v>
@@ -21691,7 +21713,7 @@
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="43"/>
+      <c r="B57" s="45"/>
       <c r="C57" s="2">
         <f>(U6+U7+U8+U9+U10+U11+U12+U13+U14+U15+U16+U17+U18+U19+U20+U21+U22+U23+U24+U25)/20</f>
         <v>17900.349999999999</v>
@@ -21712,4 +21734,441 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="46">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>100</v>
+      </c>
+      <c r="D4" s="2">
+        <v>200</v>
+      </c>
+      <c r="E4" s="2">
+        <f>1/10000000</f>
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="F4" s="2">
+        <f>(1/(300000*E4))</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="G4" s="2">
+        <f>SQRT(POWER(F4,2)+POWER(D4,2))</f>
+        <v>202.75875100994065</v>
+      </c>
+      <c r="H4" s="2">
+        <f>(1/C4)+(1/G4)</f>
+        <v>1.4931969619160719E-2</v>
+      </c>
+      <c r="I4" s="2">
+        <f>1/H4</f>
+        <v>66.970401461090503</v>
+      </c>
+      <c r="J4" s="2">
+        <f>(129+4+4+4+72+72+72+31+31+31)/10</f>
+        <v>45</v>
+      </c>
+      <c r="K4" s="2">
+        <f>((J4-I4)/I4)*100</f>
+        <v>-32.806136713776766</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="46">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>100</v>
+      </c>
+      <c r="D5" s="2">
+        <v>300</v>
+      </c>
+      <c r="E5" s="47">
+        <v>4.7000000000000003E-10</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" ref="F5:F13" si="0">(1/(300000*E5))</f>
+        <v>7092.1985815602829</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G13" si="1">SQRT(POWER(F5,2)+POWER(D5,2))</f>
+        <v>7098.5407458354211</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" ref="H5:H13" si="2">(1/C5)+(1/G5)</f>
+        <v>1.0140874024085398E-2</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" ref="I5:I13" si="3">1/H5</f>
+        <v>98.610829562118511</v>
+      </c>
+      <c r="J5" s="2">
+        <f>(21+132+132+132+23+23+23+119+119+119)/10</f>
+        <v>84.3</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" ref="K5:K13" si="4">((J5-I5)/I5)*100</f>
+        <v>-14.512431976960102</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="46">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>220</v>
+      </c>
+      <c r="D6" s="2">
+        <v>470</v>
+      </c>
+      <c r="E6" s="47">
+        <v>4.7000000000000003E-10</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>7092.1985815602829</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="1"/>
+        <v>7107.7549704731446</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="2"/>
+        <v>4.6861459457847726E-3</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="3"/>
+        <v>213.39497565147502</v>
+      </c>
+      <c r="J6" s="2">
+        <f>(228+228+228+255+255+255+282+282+282+271)/10</f>
+        <v>256.60000000000002</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="4"/>
+        <v>20.246504968837282</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="46">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2">
+        <v>220</v>
+      </c>
+      <c r="D7" s="2">
+        <v>500</v>
+      </c>
+      <c r="E7" s="2">
+        <f>1/10000000000</f>
+        <v>1E-10</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>33333.333333333336</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>33337.083122419564</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="2"/>
+        <v>4.5754511710239696E-3</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="3"/>
+        <v>218.55768155344637</v>
+      </c>
+      <c r="J7" s="2">
+        <f>(317+317+317+357+357+357+282+282+282+314)/10</f>
+        <v>318.2</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="4"/>
+        <v>45.590856261982701</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="46">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>470</v>
+      </c>
+      <c r="D8" s="2">
+        <v>570</v>
+      </c>
+      <c r="E8" s="2">
+        <f>1/10000000000</f>
+        <v>1E-10</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>33333.333333333336</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>33338.20647712038</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="2"/>
+        <v>2.1576551892797664E-3</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="3"/>
+        <v>463.46608344487322</v>
+      </c>
+      <c r="J8" s="2">
+        <f>(441+441+441+425+425+425+441+441+441+409)/10</f>
+        <v>433</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="4"/>
+        <v>-6.5735303041861091</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="46">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2">
+        <v>470</v>
+      </c>
+      <c r="D9" s="2">
+        <v>680</v>
+      </c>
+      <c r="E9" s="47">
+        <v>4.7000000000000003E-10</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>7092.1985815602829</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>7124.7232030645018</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="2"/>
+        <v>2.2680159043209948E-3</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="3"/>
+        <v>440.9140156798781</v>
+      </c>
+      <c r="J9" s="2">
+        <f>(394+394+394+326+326+326+354+354+309)/10</f>
+        <v>317.7</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="4"/>
+        <v>-27.945134719721999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="46">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2">
+        <v>680</v>
+      </c>
+      <c r="D10" s="2">
+        <v>780</v>
+      </c>
+      <c r="E10" s="2">
+        <f>1/10000000</f>
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>780.71192581586138</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="2"/>
+        <v>2.7514704236313555E-3</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="3"/>
+        <v>363.44203136307488</v>
+      </c>
+      <c r="J10" s="2">
+        <f>(354+354+354+342+342+342+362+362+362+338)/10</f>
+        <v>351.2</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="4"/>
+        <v>-3.3683587220667999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="46">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2">
+        <v>680</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="2">
+        <f>1/10000000000</f>
+        <v>1E-10</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>33333.333333333336</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
+        <v>33348.329959851231</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="2"/>
+        <v>1.5005747443997887E-3</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="3"/>
+        <v>666.41132254960587</v>
+      </c>
+      <c r="J11" s="2">
+        <f>(638+638+638+641+641+641+645+645+645+638)/10</f>
+        <v>641</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="4"/>
+        <v>-3.8131588839735415</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="46">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1360</v>
+      </c>
+      <c r="E12" s="2">
+        <f>1/10000000</f>
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="1"/>
+        <v>1360.408435401336</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="2"/>
+        <v>1.7350733603066705E-3</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="3"/>
+        <v>576.34450673788922</v>
+      </c>
+      <c r="J12" s="2">
+        <f>(590+590+590+598+598+598+607+607+607+610)/10</f>
+        <v>599.5</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="4"/>
+        <v>4.0176479503849016</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="46">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1460</v>
+      </c>
+      <c r="E13" s="2">
+        <f>1/10000000000</f>
+        <v>1E-10</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>33333.333333333336</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>33365.292012975267</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0299712647385527E-3</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="3"/>
+        <v>970.90087290332269</v>
+      </c>
+      <c r="J13" s="2">
+        <f>(993+993+993+992+992+992+991+991+991+992)/10</f>
+        <v>992</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="4"/>
+        <v>2.1731494620644192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>